<commit_message>
feat(reporting): add new Power BI dashboard with SQL logic, Excel rules, and documentation
</commit_message>
<xml_diff>
--- a/data/gold/meta_equity_model.xlsx
+++ b/data/gold/meta_equity_model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev_Environment\equity-fundamental-analytics\sandbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev_Environment\equity-fundamental-analytics\data\gold\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBB92B3-F271-46C4-8E24-5073349D034C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5D2A75-FD64-48DA-A493-C82339ACAB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{8D62F376-176E-45BA-9D0A-7FDB2C62D090}"/>
   </bookViews>
@@ -18,17 +18,18 @@
     <sheet name="dim_sector" sheetId="3" r:id="rId3"/>
     <sheet name="dim_sectorweight" sheetId="18" r:id="rId4"/>
     <sheet name="dim_metrics" sheetId="1" r:id="rId5"/>
-    <sheet name="dim_absolute" sheetId="4" r:id="rId6"/>
-    <sheet name="dim_relative" sheetId="5" r:id="rId7"/>
-    <sheet name="dim_trend" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="19" r:id="rId6"/>
+    <sheet name="dim_absolute" sheetId="4" r:id="rId7"/>
+    <sheet name="dim_relative" sheetId="5" r:id="rId8"/>
+    <sheet name="dim_trend" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">dim_absolute!$A$1:$I$397</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">dim_absolute!$A$1:$I$397</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dim_macroweight!$A$1:$E$229</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">dim_metrics!$A$1:$F$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">dim_relative!$A$1:$H$265</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">dim_relative!$A$1:$H$265</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">dim_sectorweight!$A$1:$E$628</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">dim_trend!$A$1:$G$265</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">dim_trend!$A$1:$G$265</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5910" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5933" uniqueCount="154">
   <si>
     <t>metric_id</t>
   </si>
@@ -493,6 +494,27 @@
   <si>
     <t>sector_weight</t>
   </si>
+  <si>
+    <t>revenue</t>
+  </si>
+  <si>
+    <t>Leverage</t>
+  </si>
+  <si>
+    <t>Capital Structure</t>
+  </si>
+  <si>
+    <t>Operating Efficiency</t>
+  </si>
+  <si>
+    <t>Capital Allocation</t>
+  </si>
+  <si>
+    <t>Earnings Quality</t>
+  </si>
+  <si>
+    <t>Cash Flow</t>
+  </si>
 </sst>
 </file>
 
@@ -561,7 +583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,6 +604,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15708,17 +15732,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C58B7D-0AB8-48BE-B83D-7C6A483E6E7B}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
@@ -15772,7 +15796,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>127</v>
@@ -15812,7 +15836,7 @@
         <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>127</v>
@@ -15832,7 +15856,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>127</v>
@@ -15872,7 +15896,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>127</v>
@@ -15892,7 +15916,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>127</v>
@@ -15912,7 +15936,7 @@
         <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>127</v>
@@ -15932,7 +15956,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>127</v>
@@ -16072,7 +16096,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>128</v>
@@ -16112,7 +16136,7 @@
         <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>128</v>
@@ -16132,7 +16156,7 @@
         <v>49</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>128</v>
@@ -16152,7 +16176,7 @@
         <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>128</v>
@@ -16172,7 +16196,7 @@
         <v>51</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>128</v>
@@ -16192,7 +16216,7 @@
         <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>128</v>
@@ -16232,7 +16256,7 @@
         <v>54</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>128</v>
@@ -16292,7 +16316,7 @@
         <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>129</v>
@@ -16312,7 +16336,7 @@
         <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>129</v>
@@ -16332,7 +16356,7 @@
         <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>129</v>
@@ -16352,7 +16376,7 @@
         <v>59</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>129</v>
@@ -16372,7 +16396,7 @@
         <v>60</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>129</v>
@@ -16392,7 +16416,7 @@
         <v>66</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>129</v>
@@ -16412,7 +16436,7 @@
         <v>61</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>129</v>
@@ -16432,7 +16456,7 @@
         <v>62</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>129</v>
@@ -16452,7 +16476,7 @@
         <v>63</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>129</v>
@@ -16472,7 +16496,7 @@
         <v>67</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>129</v>
@@ -16492,7 +16516,7 @@
         <v>64</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>129</v>
@@ -16532,7 +16556,7 @@
         <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>127</v>
@@ -16572,7 +16596,7 @@
         <v>71</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>127</v>
@@ -16612,7 +16636,7 @@
         <v>74</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>127</v>
@@ -16632,7 +16656,7 @@
         <v>75</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>127</v>
@@ -16652,7 +16676,7 @@
         <v>76</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>127</v>
@@ -16672,7 +16696,7 @@
         <v>77</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>127</v>
@@ -16712,7 +16736,7 @@
         <v>78</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>127</v>
@@ -16732,7 +16756,7 @@
         <v>79</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>127</v>
@@ -16752,7 +16776,7 @@
         <v>80</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>127</v>
@@ -16792,7 +16816,7 @@
         <v>97</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>128</v>
@@ -16832,7 +16856,7 @@
         <v>106</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>127</v>
@@ -16852,7 +16876,7 @@
         <v>140</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>127</v>
@@ -16872,7 +16896,7 @@
         <v>141</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>129</v>
@@ -16881,6 +16905,26 @@
         <v>2</v>
       </c>
       <c r="F58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="12">
+        <v>59</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E59" s="12">
+        <v>3</v>
+      </c>
+      <c r="F59" s="12">
         <v>1</v>
       </c>
     </row>
@@ -16891,6 +16935,105 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D980D4-422A-43B0-8F56-000EE26A52DB}">
+  <dimension ref="A2:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D41AC441-4DA4-4528-8AAF-4C00682D6EE3}">
   <dimension ref="A1:L397"/>
   <sheetViews>
@@ -33590,7 +33733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8183AB6B-9CD3-4A36-AD2A-D28B1D9F0FE6}">
   <dimension ref="A1:K265"/>
   <sheetViews>
@@ -43950,7 +44093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2D0758-1BED-4823-BF47-1AC1E8451DA8}">
   <dimension ref="A1:K265"/>
   <sheetViews>

</xml_diff>